<commit_message>
- add RNN , bi-LSTM models - fix bugs in preprocessing - update experiments scripts
</commit_message>
<xml_diff>
--- a/results/ds_stats.xlsx
+++ b/results/ds_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af91f69c463c54d7/research/twconv/twconvrsu/twconvrsu/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnny/onedrive/research/twconv/twconvrsu/twconvrsu/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{DE1FD5CC-E43B-134E-905D-5A5682820990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{823E5891-9A08-FB4B-BA9E-381290680C37}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{DE1FD5CC-E43B-134E-905D-5A5682820990}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{D2E3E04F-B40D-ED43-B463-B79C170DCD06}"/>
   <bookViews>
     <workbookView xWindow="6880" yWindow="440" windowWidth="21920" windowHeight="16580" xr2:uid="{0979E8C0-91A1-E849-B97F-24D5FF87C499}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -32,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
-    <t>pop. users</t>
-  </si>
-  <si>
     <t>conversations</t>
   </si>
   <si>
@@ -44,70 +36,73 @@
     <t>words</t>
   </si>
   <si>
-    <t>conv. threads</t>
-  </si>
-  <si>
     <t>utterances</t>
   </si>
   <si>
     <t>turns</t>
   </si>
   <si>
-    <t>min. turns</t>
-  </si>
-  <si>
-    <t>avg. turns</t>
-  </si>
-  <si>
-    <t>max. turns</t>
-  </si>
-  <si>
     <t>median turns</t>
   </si>
   <si>
     <t>users</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>timelines</t>
   </si>
   <si>
-    <t>min tweets</t>
-  </si>
-  <si>
-    <t>avg tweets</t>
-  </si>
-  <si>
-    <t>max tweets</t>
-  </si>
-  <si>
     <t>median tweet</t>
   </si>
   <si>
-    <t>min words</t>
-  </si>
-  <si>
-    <t>avg words</t>
-  </si>
-  <si>
-    <t>max words</t>
-  </si>
-  <si>
     <t>median words</t>
   </si>
   <si>
-    <t>min. context words</t>
-  </si>
-  <si>
-    <t>avg. context words</t>
-  </si>
-  <si>
-    <t>max. context words</t>
-  </si>
-  <si>
     <t>median context words</t>
+  </si>
+  <si>
+    <t>popular users</t>
+  </si>
+  <si>
+    <t>conversational threads</t>
+  </si>
+  <si>
+    <t>minimum turns</t>
+  </si>
+  <si>
+    <t>average turns</t>
+  </si>
+  <si>
+    <t>maximum turns</t>
+  </si>
+  <si>
+    <t>minimum context words</t>
+  </si>
+  <si>
+    <t>average context words</t>
+  </si>
+  <si>
+    <t>maximum context words</t>
+  </si>
+  <si>
+    <t>minimum tweets</t>
+  </si>
+  <si>
+    <t>average tweets</t>
+  </si>
+  <si>
+    <t>maximum tweets</t>
+  </si>
+  <si>
+    <t>minimum words</t>
+  </si>
+  <si>
+    <t>average words</t>
+  </si>
+  <si>
+    <t>maximum words</t>
+  </si>
+  <si>
+    <t>descriptions</t>
   </si>
 </sst>
 </file>
@@ -116,7 +111,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -150,19 +145,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="4">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -174,19 +160,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,65 +176,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -269,23 +191,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -604,7 +517,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -616,210 +529,210 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4">
+        <v>120220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>12909</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="4">
+        <v>71142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
+      <c r="C5" s="4">
+        <v>520263</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>14860508</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>588039</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>13607961</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>65274</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>345277</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>331971</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10">
-        <v>120220</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5.0858075190734402</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <v>123.61094659790299</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
-        <v>12909</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="10">
-        <v>71142</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10">
-        <v>520263</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="10">
-        <v>14860508</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10">
-        <v>588039</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="10">
-        <v>13607961</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10">
-        <v>65274</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10">
-        <v>345277</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="15">
-        <v>331971</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="8">
-        <v>5.0858075190734402</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="8">
-        <v>123.61094659790299</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5">
+        <v>68.228819999999999</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1571.7698283965001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1720</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="5">
+        <v>652282</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8">
-        <v>64</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="8">
-        <v>39436</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="9">
-        <v>4</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="9">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="12">
-        <v>5</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="8">
-        <v>68.228819999999999</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="8">
-        <v>1571.7698283965001</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1720</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="8">
-        <v>652282</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="9">
-        <v>57</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="E17" s="5">
         <v>834</v>
       </c>
     </row>

</xml_diff>